<commit_message>
Added targets for each subsystem
</commit_message>
<xml_diff>
--- a/Notes/Progress & tracking/Target tracking.xlsx
+++ b/Notes/Progress & tracking/Target tracking.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Development\Uni\Robot Programming\workspace\Autonomous_Warehouse_Project\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Development\Uni\Robot Programming\workspace\Autonomous_Warehouse_Project\Notes\Progress &amp; tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA43727-96D0-4AF6-8B4A-7FF5149F928E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="8910" xr2:uid="{368CB76C-64AE-466B-A39C-2E74A094EFEE}"/>
   </bookViews>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Target Tracking</t>
   </si>
@@ -49,13 +48,52 @@
   </si>
   <si>
     <t xml:space="preserve"> = completed</t>
+  </si>
+  <si>
+    <t>Subsystem</t>
+  </si>
+  <si>
+    <t>Job decider</t>
+  </si>
+  <si>
+    <t>Route planner</t>
+  </si>
+  <si>
+    <t>Job assignment</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Robot movement</t>
+  </si>
+  <si>
+    <t>Read file and return info</t>
+  </si>
+  <si>
+    <t>basic algorithm in place</t>
+  </si>
+  <si>
+    <t>Evenly assign jobs</t>
+  </si>
+  <si>
+    <t>Single bluetooth connection for one robot</t>
+  </si>
+  <si>
+    <t>Simplified PC  GUI</t>
+  </si>
+  <si>
+    <t>Split grid movement into behaviours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +148,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -154,17 +200,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -482,56 +530,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC08B9D-4F30-4DA7-918F-A29E981A1458}">
-  <dimension ref="B3:J8"/>
+  <dimension ref="A3:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="5" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I6" s="4"/>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="8">
+        <v>43171</v>
+      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I7" s="5"/>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="8">
+        <v>43171</v>
+      </c>
+      <c r="I7" s="4"/>
       <c r="J7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I8" s="6"/>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="8">
+        <v>43171</v>
+      </c>
+      <c r="I8" s="5"/>
       <c r="J8" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="8">
+        <v>43171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="8">
+        <v>43171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="8">
+        <v>43171</v>
       </c>
     </row>
   </sheetData>
@@ -539,5 +657,6 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'testing' into RoutePlanner"
This reverts commit 60d03ea49ab670087aefb52a920637f67dcad20a, reversing
changes made to 10916feba104872ab4e581f69a1351ab520d264e.
</commit_message>
<xml_diff>
--- a/Notes/Progress & tracking/Target tracking.xlsx
+++ b/Notes/Progress & tracking/Target tracking.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Development\Uni\Robot Programming\workspace\Autonomous_Warehouse_Project\Notes\Progress &amp; tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Development\Uni\Robot Programming\workspace\Autonomous_Warehouse_Project\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA43727-96D0-4AF6-8B4A-7FF5149F928E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="8910" xr2:uid="{368CB76C-64AE-466B-A39C-2E74A094EFEE}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Target Tracking</t>
   </si>
@@ -48,52 +49,13 @@
   </si>
   <si>
     <t xml:space="preserve"> = completed</t>
-  </si>
-  <si>
-    <t>Subsystem</t>
-  </si>
-  <si>
-    <t>Job decider</t>
-  </si>
-  <si>
-    <t>Route planner</t>
-  </si>
-  <si>
-    <t>Job assignment</t>
-  </si>
-  <si>
-    <t>Networking</t>
-  </si>
-  <si>
-    <t>GUI</t>
-  </si>
-  <si>
-    <t>Robot movement</t>
-  </si>
-  <si>
-    <t>Read file and return info</t>
-  </si>
-  <si>
-    <t>basic algorithm in place</t>
-  </si>
-  <si>
-    <t>Evenly assign jobs</t>
-  </si>
-  <si>
-    <t>Single bluetooth connection for one robot</t>
-  </si>
-  <si>
-    <t>Simplified PC  GUI</t>
-  </si>
-  <si>
-    <t>Split grid movement into behaviours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,14 +110,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -200,19 +154,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -530,126 +482,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC08B9D-4F30-4DA7-918F-A29E981A1458}">
-  <dimension ref="A3:J11"/>
+  <dimension ref="B3:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8">
-        <v>43171</v>
-      </c>
-      <c r="I6" s="3"/>
+    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I6" s="4"/>
       <c r="J6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="8">
-        <v>43171</v>
-      </c>
-      <c r="I7" s="4"/>
+    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I7" s="5"/>
       <c r="J7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="8">
-        <v>43171</v>
-      </c>
-      <c r="I8" s="5"/>
+    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I8" s="6"/>
       <c r="J8" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="8">
-        <v>43171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="8">
-        <v>43171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="8">
-        <v>43171</v>
       </c>
     </row>
   </sheetData>
@@ -657,6 +539,5 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Slight edit to target tracking
</commit_message>
<xml_diff>
--- a/Notes/Progress & tracking/Target tracking.xlsx
+++ b/Notes/Progress & tracking/Target tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Development\Uni\Robot Programming\workspace\Autonomous_Warehouse_Project\Notes\Progress &amp; tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B3321E-C2D6-4486-80BF-B756866F706A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6252B06-9063-4876-80D7-F38DAA4392D4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="8910" xr2:uid="{368CB76C-64AE-466B-A39C-2E74A094EFEE}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="A3:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
       <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="7">
         <v>43177</v>
       </c>
@@ -711,7 +711,7 @@
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="7">
         <v>43177</v>
       </c>
@@ -726,7 +726,7 @@
       <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="7">
         <v>43179</v>
       </c>

</xml_diff>